<commit_message>
minor tweaks to the functionality, and starting to add many item to category json value pairs
</commit_message>
<xml_diff>
--- a/src/categoryMatching/categories.xlsx
+++ b/src/categoryMatching/categories.xlsx
@@ -5,35 +5,22 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sebi\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sebi\receipt\src\categoryMatching\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77BB9235-E544-46F4-90DC-7841C6EA8C14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2992059-EA08-4CD7-9F37-A7E2790E1ACD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="default_1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1192" uniqueCount="613">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1390" uniqueCount="712">
   <si>
     <t>Items</t>
   </si>
@@ -1872,6 +1859,303 @@
   </si>
   <si>
     <t>ASC/MSC Sushi Box</t>
+  </si>
+  <si>
+    <t>Pfand</t>
+  </si>
+  <si>
+    <t>Rapsöl</t>
+  </si>
+  <si>
+    <t>Btl Reis-Mais.sori. 130g</t>
+  </si>
+  <si>
+    <t>Rich Knoblauchsauce 250ml</t>
+  </si>
+  <si>
+    <t>Bar. Collaz. Castell. 500g</t>
+  </si>
+  <si>
+    <t>Haribo Sft Goldbaren 160g</t>
+  </si>
+  <si>
+    <t>M. gebratene Nudeln Huhn 121g</t>
+  </si>
+  <si>
+    <t>BE Gewuerzg. 360g</t>
+  </si>
+  <si>
+    <t>Clarkys (Knabberei) 300g</t>
+  </si>
+  <si>
+    <t>Mueller FrBumi sort. 500g</t>
+  </si>
+  <si>
+    <t>Nuel. Knusperjog. sort. ab113g</t>
+  </si>
+  <si>
+    <t>Knusperjoghurt So.4 150g</t>
+  </si>
+  <si>
+    <t>Obstgarten Zero sort. 120g</t>
+  </si>
+  <si>
+    <t>Gefl. Gutsherrenbrwurstp. 200g</t>
+  </si>
+  <si>
+    <t>Bio BB Zitronensaft 0,2L</t>
+  </si>
+  <si>
+    <t>Barill. Sauce sort. 400g</t>
+  </si>
+  <si>
+    <t>Barill. Pesto sort. ab 190g</t>
+  </si>
+  <si>
+    <t>Hela CGK 500ml</t>
+  </si>
+  <si>
+    <t>Niss. Cup Nud. / Huhn 63g</t>
+  </si>
+  <si>
+    <t>Karli Knusper Dinos 400gQS</t>
+  </si>
+  <si>
+    <t>Froop sort. 150g</t>
+  </si>
+  <si>
+    <t>Stardri. Ora. 0% Zuck. EW 6x1,5L PK</t>
+  </si>
+  <si>
+    <t>Stardri. Cola-Mix 0% 6x1,5L PK</t>
+  </si>
+  <si>
+    <t>Aoste Stickado &amp; Brot sort. ab 60g</t>
+  </si>
+  <si>
+    <t>Haehnchenbrust 125g</t>
+  </si>
+  <si>
+    <t>Bernb. Pasta. Tagliatelle 500g</t>
+  </si>
+  <si>
+    <t>Leergut 1,50 EUR EW</t>
+  </si>
+  <si>
+    <t>BO-Laugenbreze 1 ST</t>
+  </si>
+  <si>
+    <t>BO-Laugenstange Kaese 1 ST</t>
+  </si>
+  <si>
+    <t>Kikkoerni. Mehrkornbrot 500g</t>
+  </si>
+  <si>
+    <t>Clarkys Stapelchips Papr. 175g</t>
+  </si>
+  <si>
+    <t>Cl. Gebaeckstangen sort. 150g</t>
+  </si>
+  <si>
+    <t>Clarkys Paprika Chips 200g</t>
+  </si>
+  <si>
+    <t>Muellermilch sort. 500ml</t>
+  </si>
+  <si>
+    <t>Paula Mini Schoko 8x50g</t>
+  </si>
+  <si>
+    <t>GL Sahne 30% 200g VLOG</t>
+  </si>
+  <si>
+    <t>Putenbrust Paprika 100g</t>
+  </si>
+  <si>
+    <t>Haehnchenbrustfilet 100g</t>
+  </si>
+  <si>
+    <t>Pri. Zugb. muellbtl. 25x60L</t>
+  </si>
+  <si>
+    <t>PrivaBackpap. Zuschn. 30ST</t>
+  </si>
+  <si>
+    <t>Mon. Ital. Nudels. Bologn. 420g</t>
+  </si>
+  <si>
+    <t>K. Fix Nat. Le. Nud. Schi. Auf. 40g</t>
+  </si>
+  <si>
+    <t>Maggi Fix Tomaten Bolognese 50g</t>
+  </si>
+  <si>
+    <t>Ma. Fix Spaghetti Bolognese 36g</t>
+  </si>
+  <si>
+    <t>BE Pfefferonen sort. ab 135g</t>
+  </si>
+  <si>
+    <t>Booster Energy sort. 0,5L DS</t>
+  </si>
+  <si>
+    <t>Knorr Knoblauchsauce 250ml</t>
+  </si>
+  <si>
+    <t>Mueller Milch sort. 400ml</t>
+  </si>
+  <si>
+    <t>Protein Mousse Choc. 200g</t>
+  </si>
+  <si>
+    <t>N.I. Mozzarella ger. 150g</t>
+  </si>
+  <si>
+    <t>Iglo Schlemmerfilet sort. 380g</t>
+  </si>
+  <si>
+    <t>HM Putenbrust 150g</t>
+  </si>
+  <si>
+    <t>Leergut 0,25 EUR EW</t>
+  </si>
+  <si>
+    <t>EW-Leergut 19%</t>
+  </si>
+  <si>
+    <t>EW-Leergut</t>
+  </si>
+  <si>
+    <t>Goesser Natur Radler 0.5L FL</t>
+  </si>
+  <si>
+    <t>MW-Pfand 0,08 EUR</t>
+  </si>
+  <si>
+    <t>Coca-Cola Zero 1x1,25L FL</t>
+  </si>
+  <si>
+    <t>EW-Pfand 0,25 EUR</t>
+  </si>
+  <si>
+    <t>GL H-Milch 1,5% 1L VL06</t>
+  </si>
+  <si>
+    <t>Bio DB Mandelmilch ungesüßt 1L</t>
+  </si>
+  <si>
+    <t>Biscotteria Schokokekssort. 125g</t>
+  </si>
+  <si>
+    <t>Haribo CRJ Chb sort. 175g</t>
+  </si>
+  <si>
+    <t>Milram Nuernberger herzhaft 150g</t>
+  </si>
+  <si>
+    <t>KW Weizenbroet. 8er 600g</t>
+  </si>
+  <si>
+    <t>Biscotteria Doppelkekssort. 500g</t>
+  </si>
+  <si>
+    <t>Liebl Sahnepudding sort. 500g</t>
+  </si>
+  <si>
+    <t>GL Naturjoghurt 4850g</t>
+  </si>
+  <si>
+    <t>N.I. Mozzarella 0bt 125g</t>
+  </si>
+  <si>
+    <t>DMH Hefe fuer 500g</t>
+  </si>
+  <si>
+    <t>GL Speisequark mager 500g</t>
+  </si>
+  <si>
+    <t>GL Sahne 30% 200g VL06</t>
+  </si>
+  <si>
+    <t>Domspitz Schmand 24% 200g</t>
+  </si>
+  <si>
+    <t>AS Sandwich Weizen 750g</t>
+  </si>
+  <si>
+    <t>BO Laugenbreze</t>
+  </si>
+  <si>
+    <t>Permanenttragetasche GRS ST</t>
+  </si>
+  <si>
+    <t>Apfel 2kg Herz für Erzeuger QS</t>
+  </si>
+  <si>
+    <t>Rucola 125g</t>
+  </si>
+  <si>
+    <t>Wiener 2x200g</t>
+  </si>
+  <si>
+    <t>KN Weizenbroet. 8er 560g</t>
+  </si>
+  <si>
+    <t>P&amp;B 2-Klingen Rasiererset 20ST</t>
+  </si>
+  <si>
+    <t>Clarkys Trockenpflaumen 500g</t>
+  </si>
+  <si>
+    <t>BioKraeuter/Chili sort. 40g</t>
+  </si>
+  <si>
+    <t>Fevora Topa P4 10x200BL</t>
+  </si>
+  <si>
+    <t>Taschentuecher Box 100ST</t>
+  </si>
+  <si>
+    <t>Einmalhandschuhe 1 100ST</t>
+  </si>
+  <si>
+    <t>BE Apfelmus o. Zuckerz. 710g</t>
+  </si>
+  <si>
+    <t>Priva Geschirrreiniger 6ST</t>
+  </si>
+  <si>
+    <t>Corny Haferkraft Kakao 140g</t>
+  </si>
+  <si>
+    <t>GL Gouda jung HF3 SHB 400g</t>
+  </si>
+  <si>
+    <t>VL Eier BH 10ST</t>
+  </si>
+  <si>
+    <t>Clarkys Walnusskerne 200g</t>
+  </si>
+  <si>
+    <t>SammelNr. Metzgerei</t>
+  </si>
+  <si>
+    <t>Aprikosen 1kg</t>
+  </si>
+  <si>
+    <t>Grapefruit rose ST</t>
+  </si>
+  <si>
+    <t>Rispentomaten</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bananen Lose </t>
+  </si>
+  <si>
+    <t>Plattpfirsiche 500g</t>
+  </si>
+  <si>
+    <t>Potato Pommes WS 1kg</t>
   </si>
 </sst>
 </file>
@@ -2243,16 +2527,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B596"/>
+  <dimension ref="A1:B695"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="A677" zoomScale="265" zoomScaleNormal="265" workbookViewId="0">
+      <selection activeCell="B696" sqref="B696"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.5703125" customWidth="1"/>
-    <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -7023,6 +7306,798 @@
         <v>12</v>
       </c>
     </row>
+    <row r="597" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A597" t="s">
+        <v>613</v>
+      </c>
+      <c r="B597" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="598" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A598" t="s">
+        <v>614</v>
+      </c>
+      <c r="B598" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="599" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A599" t="s">
+        <v>615</v>
+      </c>
+      <c r="B599" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="600" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A600" t="s">
+        <v>616</v>
+      </c>
+      <c r="B600" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="601" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A601" t="s">
+        <v>617</v>
+      </c>
+      <c r="B601" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="602" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A602" t="s">
+        <v>618</v>
+      </c>
+      <c r="B602" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="603" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A603" t="s">
+        <v>619</v>
+      </c>
+      <c r="B603" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="604" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A604" t="s">
+        <v>620</v>
+      </c>
+      <c r="B604" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="605" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A605" t="s">
+        <v>621</v>
+      </c>
+      <c r="B605" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="606" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A606" t="s">
+        <v>622</v>
+      </c>
+      <c r="B606" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="607" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A607" t="s">
+        <v>623</v>
+      </c>
+      <c r="B607" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="608" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A608" t="s">
+        <v>624</v>
+      </c>
+      <c r="B608" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="609" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A609" t="s">
+        <v>625</v>
+      </c>
+      <c r="B609" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="610" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A610" t="s">
+        <v>626</v>
+      </c>
+      <c r="B610" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="611" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A611" t="s">
+        <v>627</v>
+      </c>
+      <c r="B611" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="612" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A612" t="s">
+        <v>628</v>
+      </c>
+      <c r="B612" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="613" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A613" t="s">
+        <v>629</v>
+      </c>
+      <c r="B613" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="614" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A614" t="s">
+        <v>630</v>
+      </c>
+      <c r="B614" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="615" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A615" t="s">
+        <v>631</v>
+      </c>
+      <c r="B615" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="616" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A616" t="s">
+        <v>632</v>
+      </c>
+      <c r="B616" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="617" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A617" t="s">
+        <v>633</v>
+      </c>
+      <c r="B617" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="618" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A618" t="s">
+        <v>634</v>
+      </c>
+      <c r="B618" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="619" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A619" t="s">
+        <v>635</v>
+      </c>
+      <c r="B619" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="620" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A620" t="s">
+        <v>636</v>
+      </c>
+      <c r="B620" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="621" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A621" t="s">
+        <v>637</v>
+      </c>
+      <c r="B621" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="622" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A622" t="s">
+        <v>638</v>
+      </c>
+      <c r="B622" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="623" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A623" t="s">
+        <v>639</v>
+      </c>
+      <c r="B623" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="624" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A624" t="s">
+        <v>640</v>
+      </c>
+      <c r="B624" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="625" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A625" t="s">
+        <v>641</v>
+      </c>
+      <c r="B625" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="626" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A626" t="s">
+        <v>642</v>
+      </c>
+      <c r="B626" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="627" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A627" t="s">
+        <v>643</v>
+      </c>
+      <c r="B627" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="628" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A628" t="s">
+        <v>644</v>
+      </c>
+      <c r="B628" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="629" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A629" t="s">
+        <v>711</v>
+      </c>
+      <c r="B629" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="630" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A630" t="s">
+        <v>645</v>
+      </c>
+      <c r="B630" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="631" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A631" t="s">
+        <v>646</v>
+      </c>
+      <c r="B631" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="632" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A632" t="s">
+        <v>647</v>
+      </c>
+      <c r="B632" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="633" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A633" t="s">
+        <v>648</v>
+      </c>
+      <c r="B633" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="634" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A634" t="s">
+        <v>649</v>
+      </c>
+      <c r="B634" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="635" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A635" t="s">
+        <v>650</v>
+      </c>
+      <c r="B635" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="636" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A636" t="s">
+        <v>651</v>
+      </c>
+      <c r="B636" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="637" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A637" t="s">
+        <v>652</v>
+      </c>
+      <c r="B637" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="638" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A638" t="s">
+        <v>653</v>
+      </c>
+      <c r="B638" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="639" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A639" t="s">
+        <v>654</v>
+      </c>
+      <c r="B639" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="640" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A640" t="s">
+        <v>655</v>
+      </c>
+      <c r="B640" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="641" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A641" t="s">
+        <v>656</v>
+      </c>
+      <c r="B641" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="642" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A642" t="s">
+        <v>657</v>
+      </c>
+      <c r="B642" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="643" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A643" t="s">
+        <v>658</v>
+      </c>
+      <c r="B643" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="644" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A644" t="s">
+        <v>659</v>
+      </c>
+      <c r="B644" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="645" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A645" t="s">
+        <v>660</v>
+      </c>
+      <c r="B645" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="646" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A646" t="s">
+        <v>661</v>
+      </c>
+      <c r="B646" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="647" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A647" t="s">
+        <v>662</v>
+      </c>
+      <c r="B647" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="648" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A648" t="s">
+        <v>663</v>
+      </c>
+      <c r="B648" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="649" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A649" t="s">
+        <v>664</v>
+      </c>
+      <c r="B649" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="650" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A650" t="s">
+        <v>665</v>
+      </c>
+      <c r="B650" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="651" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A651" t="s">
+        <v>666</v>
+      </c>
+      <c r="B651" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="652" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A652" t="s">
+        <v>667</v>
+      </c>
+      <c r="B652" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="653" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A653" t="s">
+        <v>668</v>
+      </c>
+      <c r="B653" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="654" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A654" t="s">
+        <v>669</v>
+      </c>
+      <c r="B654" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="655" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A655" t="s">
+        <v>670</v>
+      </c>
+      <c r="B655" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="656" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A656" t="s">
+        <v>671</v>
+      </c>
+      <c r="B656" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="657" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A657" t="s">
+        <v>672</v>
+      </c>
+      <c r="B657" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="658" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A658" t="s">
+        <v>673</v>
+      </c>
+      <c r="B658" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="659" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A659" t="s">
+        <v>674</v>
+      </c>
+      <c r="B659" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="660" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A660" t="s">
+        <v>675</v>
+      </c>
+      <c r="B660" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="661" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A661" t="s">
+        <v>676</v>
+      </c>
+      <c r="B661" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="662" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A662" t="s">
+        <v>677</v>
+      </c>
+      <c r="B662" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="663" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A663" t="s">
+        <v>678</v>
+      </c>
+      <c r="B663" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="664" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A664" t="s">
+        <v>679</v>
+      </c>
+      <c r="B664" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="665" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A665" t="s">
+        <v>680</v>
+      </c>
+      <c r="B665" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="666" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A666" t="s">
+        <v>681</v>
+      </c>
+      <c r="B666" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="667" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A667" t="s">
+        <v>682</v>
+      </c>
+      <c r="B667" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="668" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A668" t="s">
+        <v>683</v>
+      </c>
+      <c r="B668" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="669" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A669" t="s">
+        <v>684</v>
+      </c>
+      <c r="B669" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="670" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A670" t="s">
+        <v>685</v>
+      </c>
+      <c r="B670" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="671" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A671" t="s">
+        <v>686</v>
+      </c>
+      <c r="B671" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="672" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A672" t="s">
+        <v>687</v>
+      </c>
+      <c r="B672" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="673" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A673" t="s">
+        <v>688</v>
+      </c>
+      <c r="B673" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="674" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A674" t="s">
+        <v>689</v>
+      </c>
+      <c r="B674" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="675" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A675" t="s">
+        <v>690</v>
+      </c>
+      <c r="B675" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="676" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A676" t="s">
+        <v>691</v>
+      </c>
+      <c r="B676" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="677" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A677" t="s">
+        <v>692</v>
+      </c>
+      <c r="B677" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="678" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A678" t="s">
+        <v>693</v>
+      </c>
+      <c r="B678" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="679" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A679" t="s">
+        <v>694</v>
+      </c>
+      <c r="B679" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="680" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A680" t="s">
+        <v>695</v>
+      </c>
+      <c r="B680" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="681" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A681" t="s">
+        <v>696</v>
+      </c>
+      <c r="B681" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="682" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A682" t="s">
+        <v>697</v>
+      </c>
+      <c r="B682" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="683" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A683" t="s">
+        <v>698</v>
+      </c>
+      <c r="B683" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="684" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A684" t="s">
+        <v>699</v>
+      </c>
+      <c r="B684" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="685" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A685" t="s">
+        <v>700</v>
+      </c>
+      <c r="B685" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="686" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A686" t="s">
+        <v>701</v>
+      </c>
+      <c r="B686" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="687" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A687" t="s">
+        <v>702</v>
+      </c>
+      <c r="B687" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="688" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A688" t="s">
+        <v>703</v>
+      </c>
+      <c r="B688" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="689" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A689" t="s">
+        <v>704</v>
+      </c>
+      <c r="B689" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="690" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A690" t="s">
+        <v>705</v>
+      </c>
+      <c r="B690" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="691" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A691" t="s">
+        <v>706</v>
+      </c>
+      <c r="B691" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="692" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A692" t="s">
+        <v>707</v>
+      </c>
+      <c r="B692" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="693" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A693" t="s">
+        <v>708</v>
+      </c>
+      <c r="B693" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="694" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A694" t="s">
+        <v>709</v>
+      </c>
+      <c r="B694" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="695" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A695" t="s">
+        <v>710</v>
+      </c>
+      <c r="B695" t="s">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>